<commit_message>
mark red in template.xlsx
</commit_message>
<xml_diff>
--- a/i2up/excel/rule_auto.xlsx
+++ b/i2up/excel/rule_auto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A51CB9D-39AB-294D-B2E9-30DE74A2E91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1547D4-DFF1-EF4E-A9C0-A1C37A03107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="28140" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_u" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="136">
   <si>
     <t>{</t>
   </si>
@@ -308,9 +308,6 @@
     <t>192.168.55.250</t>
   </si>
   <si>
-    <t>192.168.55.252</t>
-  </si>
-  <si>
     <t>manga</t>
   </si>
   <si>
@@ -431,13 +428,7 @@
     <t>export</t>
   </si>
   <si>
-    <t>credential</t>
-  </si>
-  <si>
     <t>portfolio</t>
-  </si>
-  <si>
-    <t>192.168.55.254</t>
   </si>
   <si>
     <t>asset</t>
@@ -804,9 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2071,22 +2060,22 @@
         <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
-      </c>
-      <c r="H1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2094,25 +2083,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
         <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
       </c>
       <c r="D2">
         <v>26804</v>
       </c>
       <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2125,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2168,7 +2157,7 @@
         <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I1" t="s">
         <v>84</v>
@@ -2202,90 +2191,65 @@
       <c r="G2">
         <v>3306</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="J2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G3">
         <v>3306</v>
       </c>
-      <c r="H3" t="s">
-        <v>134</v>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" t="s">
+        <v>93</v>
       </c>
       <c r="K3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="G4">
-        <v>3306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5">
-        <v>3306</v>
-      </c>
-      <c r="I5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6">
         <v>9092</v>
       </c>
     </row>
@@ -2325,49 +2289,49 @@
         <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>119</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>121</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" t="s">
         <v>122</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" t="s">
         <v>125</v>
-      </c>
-      <c r="N1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" t="s">
-        <v>124</v>
-      </c>
-      <c r="P1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2375,28 +2339,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" t="s">
         <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" t="s">
-        <v>130</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -2405,13 +2369,13 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M2" t="s">
         <v>131</v>
       </c>
-      <c r="M2" t="s">
-        <v>132</v>
-      </c>
       <c r="N2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -2419,16 +2383,16 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -2436,28 +2400,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2466,13 +2430,13 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M4" t="s">
         <v>131</v>
       </c>
-      <c r="M4" t="s">
-        <v>132</v>
-      </c>
       <c r="N4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O4">
         <v>1</v>

</xml_diff>

<commit_message>
add generate_db_json() to json_tool
</commit_message>
<xml_diff>
--- a/i2up/excel/rule_auto.xlsx
+++ b/i2up/excel/rule_auto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1547D4-DFF1-EF4E-A9C0-A1C37A03107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A048CC-F471-2840-A14B-8AE2683E3788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="28140" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_u" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="135">
   <si>
     <t>{</t>
   </si>
@@ -302,9 +302,6 @@
     <t>mysql</t>
   </si>
   <si>
-    <t>soure|target</t>
-  </si>
-  <si>
     <t>192.168.55.250</t>
   </si>
   <si>
@@ -431,10 +428,10 @@
     <t>portfolio</t>
   </si>
   <si>
-    <t>asset</t>
-  </si>
-  <si>
-    <t>msq_u_c1_2</t>
+    <t>msq_test</t>
+  </si>
+  <si>
+    <t>source|target</t>
   </si>
 </sst>
 </file>
@@ -795,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2060,22 +2057,22 @@
         <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2083,25 +2080,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
       </c>
       <c r="D2">
         <v>26804</v>
       </c>
       <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>107</v>
-      </c>
-      <c r="H2" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2116,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2126,6 +2123,7 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
@@ -2157,7 +2155,7 @@
         <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I1" t="s">
         <v>84</v>
@@ -2183,19 +2181,19 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
       </c>
       <c r="G2">
         <v>3306</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2203,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>89</v>
@@ -2212,22 +2210,22 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3">
         <v>3306</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2235,19 +2233,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>89</v>
       </c>
       <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="E4" t="s">
-        <v>98</v>
-      </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4">
         <v>9092</v>
@@ -2261,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76AAA83-80DE-C04C-95F4-C95AE871C727}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2289,49 +2287,49 @@
         <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>117</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>118</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>119</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>120</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" t="s">
         <v>121</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" t="s">
         <v>124</v>
-      </c>
-      <c r="N1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2339,43 +2337,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N2" t="s">
         <v>128</v>
-      </c>
-      <c r="I2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>130</v>
-      </c>
-      <c r="M2" t="s">
-        <v>131</v>
-      </c>
-      <c r="N2" t="s">
-        <v>129</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -2383,16 +2381,16 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -2400,28 +2398,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2430,16 +2422,24 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" t="s">
         <v>130</v>
       </c>
-      <c r="M4" t="s">
-        <v>131</v>
-      </c>
       <c r="N4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use chinese head instead
</commit_message>
<xml_diff>
--- a/i2up/excel/rule_auto.xlsx
+++ b/i2up/excel/rule_auto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A048CC-F471-2840-A14B-8AE2683E3788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4CA6C2-43C6-A249-B66A-2E44EFA73825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_u" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
   <si>
     <t>{</t>
   </si>
@@ -263,39 +263,9 @@
     <t>"tgt_db_name":</t>
   </si>
   <si>
-    <t>NO.</t>
-  </si>
-  <si>
-    <t>node_name</t>
-  </si>
-  <si>
-    <t>db_type</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>port</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>passwd</t>
-  </si>
-  <si>
-    <t>defalut_db</t>
-  </si>
-  <si>
     <t>msq_u_auto</t>
   </si>
   <si>
-    <t>db_name</t>
-  </si>
-  <si>
     <t>centos1</t>
   </si>
   <si>
@@ -314,27 +284,6 @@
     <t>192.168.55.11</t>
   </si>
   <si>
-    <t>kfk_u_auto</t>
-  </si>
-  <si>
-    <t>kafka</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>data_port</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>node_type</t>
-  </si>
-  <si>
     <t>hadoop3</t>
   </si>
   <si>
@@ -350,63 +299,6 @@
     <t>Info@1234</t>
   </si>
   <si>
-    <t>src|tgt</t>
-  </si>
-  <si>
-    <t>log_dir</t>
-  </si>
-  <si>
-    <t>cache_dir</t>
-  </si>
-  <si>
-    <t>mysql_name</t>
-  </si>
-  <si>
-    <t>src_db_name</t>
-  </si>
-  <si>
-    <t>src_db</t>
-  </si>
-  <si>
-    <t>src_table</t>
-  </si>
-  <si>
-    <t>tgt_db_name</t>
-  </si>
-  <si>
-    <t>dst_db</t>
-  </si>
-  <si>
-    <t>dst_table</t>
-  </si>
-  <si>
-    <t>full_sync</t>
-  </si>
-  <si>
-    <t>dump_thd</t>
-  </si>
-  <si>
-    <t>load_thd</t>
-  </si>
-  <si>
-    <t>existing_table</t>
-  </si>
-  <si>
-    <t>incre_sync</t>
-  </si>
-  <si>
-    <t>dyn_thread</t>
-  </si>
-  <si>
-    <t>full_sync_custom_cfg</t>
-  </si>
-  <si>
-    <t>incre_full_sync_custom_cfg</t>
-  </si>
-  <si>
-    <t>cred_name</t>
-  </si>
-  <si>
     <t>msq_u_c1_auto</t>
   </si>
   <si>
@@ -431,14 +323,342 @@
     <t>msq_test</t>
   </si>
   <si>
-    <t>source|target</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>序号</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>名称</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数据库类型</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>地址</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>端口</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>凭据名称</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>用户名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>密码</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>默认数据库</t>
+    </r>
+  </si>
+  <si>
+    <t>所有者</t>
+  </si>
+  <si>
+    <t>源库|备库</t>
+  </si>
+  <si>
+    <t>备库</t>
+  </si>
+  <si>
+    <t>数据库类型</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>工作节点</t>
+  </si>
+  <si>
+    <t>角色</t>
+  </si>
+  <si>
+    <t>序号</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数据端口</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数据缓存目录</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日志目录</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>口令</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>节点类型</t>
+    </r>
+  </si>
+  <si>
+    <t>源端节点|备端节点</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备端数据库</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备端库名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备端表名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全量装载线程数</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表覆盖策略</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>增量同步</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>操作装载时间和日期</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>操作装载标记</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>所有者</t>
+    </r>
+  </si>
+  <si>
+    <t>全量自定义配置</t>
+  </si>
+  <si>
+    <t>增量自定义配置</t>
+  </si>
+  <si>
+    <t>源端数据库</t>
+  </si>
+  <si>
+    <t>源端库名</t>
+  </si>
+  <si>
+    <t>源端表名</t>
+  </si>
+  <si>
+    <t>全量同步</t>
+  </si>
+  <si>
+    <t>增量装载线程数</t>
+  </si>
+  <si>
+    <t>全量导出线程数</t>
+  </si>
+  <si>
+    <t>规则名称</t>
+  </si>
+  <si>
+    <t>cdc_upd_tmstamp</t>
+  </si>
+  <si>
+    <t>cdc_upd_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +681,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -470,7 +702,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -478,15 +710,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -792,9 +1047,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -803,12 +1060,12 @@
     <col min="5" max="5" width="1.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -816,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -827,7 +1084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -835,12 +1092,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -851,7 +1108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -859,17 +1116,17 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -877,7 +1134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -885,17 +1142,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="C13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -903,12 +1160,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="C15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="C16" t="s">
         <v>17</v>
       </c>
@@ -919,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="C17" t="s">
         <v>19</v>
       </c>
@@ -930,7 +1187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="C18" t="s">
         <v>20</v>
       </c>
@@ -938,22 +1195,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="C20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -964,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -975,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -983,7 +1240,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1001,7 +1258,7 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -1010,12 +1267,12 @@
     <col min="5" max="5" width="1.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1023,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1034,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1042,12 +1299,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1066,17 +1323,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -1084,17 +1341,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1102,12 +1359,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="C14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -1118,7 +1375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1129,7 +1386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="C17" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="C18" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="C19" t="s">
         <v>35</v>
       </c>
@@ -1162,7 +1419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="C21" t="s">
         <v>37</v>
       </c>
@@ -1184,7 +1441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="C22" t="s">
         <v>20</v>
       </c>
@@ -1192,22 +1449,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="C23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="C24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1218,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +1486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +1494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1255,7 +1512,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
@@ -1263,12 +1520,12 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1276,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1295,12 +1552,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1319,17 +1576,17 @@
         <v>9092</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -1337,22 +1594,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="C12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1363,7 +1620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1382,7 +1639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1657,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -1409,12 +1666,12 @@
     <col min="5" max="5" width="1.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1422,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1433,7 +1690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -1441,12 +1698,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1457,7 +1714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1468,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1479,7 +1736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1490,7 +1747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1501,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1512,7 +1769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1523,7 +1780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1531,12 +1788,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="B15" t="s">
         <v>56</v>
       </c>
@@ -1544,12 +1801,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="C16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="C17" t="s">
         <v>57</v>
       </c>
@@ -1560,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="C18" t="s">
         <v>59</v>
       </c>
@@ -1568,17 +1825,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="C20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>60</v>
       </c>
@@ -1589,7 +1846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -1600,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="B23" t="s">
         <v>63</v>
       </c>
@@ -1611,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -1619,17 +1876,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1640,7 +1897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1648,7 +1905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1666,7 +1923,7 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -1675,12 +1932,12 @@
     <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1688,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>67</v>
       </c>
@@ -1696,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="C4" t="s">
         <v>68</v>
       </c>
@@ -1707,7 +1964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="C5" t="s">
         <v>69</v>
       </c>
@@ -1718,7 +1975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="C6" t="s">
         <v>70</v>
       </c>
@@ -1726,12 +1983,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="D7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="D8" t="s">
         <v>56</v>
       </c>
@@ -1742,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="D9" t="s">
         <v>60</v>
       </c>
@@ -1753,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="D10" t="s">
         <v>61</v>
       </c>
@@ -1764,7 +2021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="D11" t="s">
         <v>63</v>
       </c>
@@ -1775,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="D12" t="s">
         <v>64</v>
       </c>
@@ -1783,17 +2040,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="D13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="D14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="C15" t="s">
         <v>72</v>
       </c>
@@ -1801,17 +2058,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="C16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1822,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1833,7 +2090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1844,7 +2101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1855,7 +2112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +2123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1874,17 +2131,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="B24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="B25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1895,7 +2152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1906,7 +2163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1917,7 +2174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1925,12 +2182,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="B30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="B31" t="s">
         <v>56</v>
       </c>
@@ -1941,7 +2198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="B32" t="s">
         <v>60</v>
       </c>
@@ -1952,7 +2209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="B33" t="s">
         <v>61</v>
       </c>
@@ -1963,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="B34" t="s">
         <v>63</v>
       </c>
@@ -1974,7 +2231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="B35" t="s">
         <v>64</v>
       </c>
@@ -1982,17 +2239,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="B36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="B37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -2003,7 +2260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2014,7 +2271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -2022,7 +2279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2036,69 +2293,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA53CE64-CEB5-8542-B539-0B6E7451096E}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D2">
         <v>26804</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2106,149 +2363,149 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{7FDEB728-D3FF-ED41-8A3E-2CBDADD5B886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H2" s="5">
+        <v>3306</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2">
+      <c r="H3" s="5">
         <v>3306</v>
       </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3">
-        <v>3306</v>
-      </c>
-      <c r="I3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4">
-        <v>9092</v>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2259,13 +2516,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76AAA83-80DE-C04C-95F4-C95AE871C727}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -2273,92 +2530,103 @@
     <col min="5" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
+        <v>123</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" t="s">
-        <v>118</v>
+        <v>125</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="K1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="L1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="N1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" t="s">
         <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" t="s">
-        <v>128</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -2367,53 +2635,62 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="M2" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R2" t="s">
+        <v>142</v>
+      </c>
+      <c r="S2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="E3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" t="s">
         <v>92</v>
-      </c>
-      <c r="F4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>128</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2422,24 +2699,27 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="M4" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="N4" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="E5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" t="s">
-        <v>132</v>
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add get_kfks() and get_msq_kfk_rules() to excel_tool
</commit_message>
<xml_diff>
--- a/i2up/excel/rule_auto.xlsx
+++ b/i2up/excel/rule_auto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4CA6C2-43C6-A249-B66A-2E44EFA73825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C753CB-1236-9A4E-8842-9C7186901177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="28140" windowHeight="15180" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="620" windowWidth="28140" windowHeight="15180" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_u" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,16 @@
     <sheet name="msq_u_kfk" sheetId="5" r:id="rId5"/>
     <sheet name="work_node" sheetId="7" r:id="rId6"/>
     <sheet name="db_node" sheetId="9" r:id="rId7"/>
-    <sheet name="msq_rule" sheetId="8" r:id="rId8"/>
+    <sheet name="kfk_node" sheetId="10" r:id="rId8"/>
+    <sheet name="msq_msq_rule" sheetId="8" r:id="rId9"/>
+    <sheet name="msq_kfk_rule" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="154">
   <si>
     <t>{</t>
   </si>
@@ -431,16 +433,7 @@
     <t>所有者</t>
   </si>
   <si>
-    <t>源库|备库</t>
-  </si>
-  <si>
     <t>备库</t>
-  </si>
-  <si>
-    <t>数据库类型</t>
-  </si>
-  <si>
-    <t>MySQL</t>
   </si>
   <si>
     <t>工作节点</t>
@@ -652,6 +645,81 @@
   </si>
   <si>
     <t>cdc_upd_type</t>
+  </si>
+  <si>
+    <t>kfk_u_auto</t>
+  </si>
+  <si>
+    <t>kafka</t>
+  </si>
+  <si>
+    <t>身份认证</t>
+  </si>
+  <si>
+    <r>
+      <t>kafka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>凭证</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>kafka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>服务名</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>keytab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>路径</t>
+    </r>
+  </si>
+  <si>
+    <t>kerberos</t>
+  </si>
+  <si>
+    <t>root/kafka_keytab</t>
+  </si>
+  <si>
+    <t>kafka@sdp1-xyk</t>
+  </si>
+  <si>
+    <t>备端topic</t>
+  </si>
+  <si>
+    <t>备端自动建表</t>
+  </si>
+  <si>
+    <t>dump.no.data=true</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>msq_u_kfk_auto</t>
   </si>
 </sst>
 </file>
@@ -702,7 +770,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -725,23 +793,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1250,6 +1349,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F785585-F36B-294D-B818-49D5E8C12014}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="C4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E29"/>
@@ -1509,7 +1749,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1919,7 +2159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -2293,7 +2533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA53CE64-CEB5-8542-B539-0B6E7451096E}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2308,28 +2550,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
         <v>102</v>
       </c>
       <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2355,7 +2597,7 @@
         <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2369,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C49F8E9-B962-1843-8F78-FE23AAE2A24E}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2382,16 +2624,15 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>99</v>
       </c>
@@ -2399,40 +2640,37 @@
         <v>100</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2445,31 +2683,26 @@
       <c r="D2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="5">
+      <c r="G2" s="5">
         <v>3306</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>82</v>
       </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="L2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M2" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2483,18 +2716,18 @@
         <v>80</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="5">
+      <c r="G3" s="5">
         <v>3306</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="J3" s="5" t="s">
         <v>82</v>
       </c>
@@ -2502,9 +2735,6 @@
         <v>82</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M3" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2515,11 +2745,123 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00E08A5-ABC4-3947-A76D-AB94C6311FFD}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="5">
+        <v>9092</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="E15" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{F95E29FD-AA1D-C04A-A2FE-536CAA040B26}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76AAA83-80DE-C04C-95F4-C95AE871C727}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2546,58 +2888,58 @@
         <v>99</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="L1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="P1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" t="s">
         <v>126</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>129</v>
-      </c>
-      <c r="R1" t="s">
-        <v>130</v>
-      </c>
-      <c r="S1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -2647,10 +2989,10 @@
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="R2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="S2" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
add create_all_objects() to excel_tool
</commit_message>
<xml_diff>
--- a/i2up/excel/rule_auto.xlsx
+++ b/i2up/excel/rule_auto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/i2up/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C753CB-1236-9A4E-8842-9C7186901177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8943D-9D8F-554B-B854-5862BAE2716A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="620" windowWidth="28140" windowHeight="15180" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="520" windowWidth="28140" windowHeight="15180" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msq_u" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="152">
   <si>
     <t>{</t>
   </si>
@@ -698,15 +698,6 @@
     </r>
   </si>
   <si>
-    <t>kerberos</t>
-  </si>
-  <si>
-    <t>root/kafka_keytab</t>
-  </si>
-  <si>
-    <t>kafka@sdp1-xyk</t>
-  </si>
-  <si>
     <t>备端topic</t>
   </si>
   <si>
@@ -720,6 +711,9 @@
   </si>
   <si>
     <t>msq_u_kfk_auto</t>
+  </si>
+  <si>
+    <t>源库|备库</t>
   </si>
 </sst>
 </file>
@@ -822,7 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,13 +828,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1353,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F785585-F36B-294D-B818-49D5E8C12014}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1393,13 +1386,13 @@
         <v>133</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>134</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>136</v>
@@ -1428,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>78</v>
@@ -1458,10 +1451,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -2614,7 +2607,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2683,7 +2676,9 @@
       <c r="D2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F2" s="5" t="s">
         <v>81</v>
       </c>
@@ -2748,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00E08A5-ABC4-3947-A76D-AB94C6311FFD}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2793,7 +2788,7 @@
       <c r="H1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>143</v>
       </c>
       <c r="J1" s="7" t="s">
@@ -2828,18 +2823,10 @@
       <c r="G2" s="5">
         <v>9092</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>147</v>
-      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
         <v>98</v>
       </c>
@@ -2848,9 +2835,6 @@
       <c r="E15" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{F95E29FD-AA1D-C04A-A2FE-536CAA040B26}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>